<commit_message>
crf labelling for andrea
</commit_message>
<xml_diff>
--- a/crf_template.xlsx
+++ b/crf_template.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tbarfoot/Documents/MALIMAR_labseg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D281B2FD-D609-DC47-8E95-C65A8FC03355}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF6ED731-B955-D749-BB51-434CA320B8E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12280" yWindow="5320" windowWidth="19460" windowHeight="19460" xr2:uid="{3B8CEF8C-2797-2840-83D1-1B369CABCF20}"/>
+    <workbookView xWindow="6740" yWindow="460" windowWidth="25020" windowHeight="19420" xr2:uid="{3B8CEF8C-2797-2840-83D1-1B369CABCF20}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="scores" sheetId="2" r:id="rId2"/>
+    <sheet name="crf" sheetId="1" r:id="rId1"/>
+    <sheet name="drop down options" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
   <si>
     <t>Score</t>
   </si>
@@ -137,6 +137,24 @@
   </si>
   <si>
     <t>Normal</t>
+  </si>
+  <si>
+    <t>Scan Date</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Disease Pattern</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Artefact?</t>
   </si>
 </sst>
 </file>
@@ -160,7 +178,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -302,11 +320,143 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -336,6 +486,52 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -652,10 +848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55B4468A-E7FA-3343-886E-800207109A43}">
-  <dimension ref="A3:G22"/>
+  <dimension ref="A3:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,7 +862,7 @@
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C3" s="16" t="s">
         <v>19</v>
       </c>
@@ -678,8 +874,11 @@
       <c r="G3" s="19" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>35</v>
       </c>
@@ -694,8 +893,9 @@
       </c>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="36"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -718,8 +918,9 @@
         <f t="shared" ref="G5:G22" si="0">IF(AND(C5 = 0, D5=0, E5="No", F5="No"), "Yes", "No")</f>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -742,8 +943,9 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -766,8 +968,9 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -790,8 +993,9 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="8"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -814,8 +1018,9 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="8"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -838,8 +1043,9 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -862,8 +1068,9 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -886,8 +1093,9 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -910,8 +1118,9 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -934,8 +1143,9 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -958,8 +1168,9 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" s="8"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -982,8 +1193,9 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="8"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1006,8 +1218,9 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="8"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1030,8 +1243,9 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1054,8 +1268,9 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1078,8 +1293,9 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="8"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1102,8 +1318,9 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="8"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1126,12 +1343,82 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
+      <c r="H22" s="9"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="24"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="26"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="27"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="30"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="27"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="30"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="31"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="10">
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="C30:G33"/>
+    <mergeCell ref="H3:H4"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1139,25 +1426,25 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DED3B03D-BD96-C44A-BF5E-79A174F118F8}">
           <x14:formula1>
-            <xm:f>scores!$A$2:$A$6</xm:f>
+            <xm:f>'drop down options'!$A$2:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>C5:C22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A4589627-856D-C647-9913-6BB245FDC873}">
           <x14:formula1>
-            <xm:f>scores!$C$2:$C$6</xm:f>
+            <xm:f>'drop down options'!$C$2:$C$6</xm:f>
           </x14:formula1>
           <xm:sqref>D5:D22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5883C33D-C99E-A645-AA97-74602DEEA8B7}">
           <x14:formula1>
-            <xm:f>scores!$F$2:$F$3</xm:f>
+            <xm:f>'drop down options'!$F$2:$F$3</xm:f>
           </x14:formula1>
           <xm:sqref>E5:E22</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7EA332CE-95FD-0049-80C2-13A238BA7B6A}">
           <x14:formula1>
-            <xm:f>scores!$G$2:$G$3</xm:f>
+            <xm:f>'drop down options'!$G$2:$G$3</xm:f>
           </x14:formula1>
           <xm:sqref>F5:F22</xm:sqref>
         </x14:dataValidation>
@@ -1172,7 +1459,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
crf labelling for andrea updated
</commit_message>
<xml_diff>
--- a/crf_template.xlsx
+++ b/crf_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tbarfoot/Documents/MALIMAR_labseg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF6ED731-B955-D749-BB51-434CA320B8E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F5E57D-6C7E-034C-9B8C-10ACEC5E4EB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6740" yWindow="460" windowWidth="25020" windowHeight="19420" xr2:uid="{3B8CEF8C-2797-2840-83D1-1B369CABCF20}"/>
+    <workbookView xWindow="-3040" yWindow="-21960" windowWidth="14080" windowHeight="15920" xr2:uid="{3B8CEF8C-2797-2840-83D1-1B369CABCF20}"/>
   </bookViews>
   <sheets>
     <sheet name="crf" sheetId="1" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>1 to 4</t>
   </si>
   <si>
-    <t>&gt;5</t>
-  </si>
-  <si>
     <t>&gt;10</t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>Artefact?</t>
+  </si>
+  <si>
+    <t>5 to 10</t>
   </si>
 </sst>
 </file>
@@ -473,21 +473,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -495,6 +480,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -504,9 +495,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -516,9 +504,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -532,6 +517,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -850,9 +850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55B4468A-E7FA-3343-886E-800207109A43}">
   <dimension ref="A3:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -863,37 +861,37 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="19" t="s">
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="35" t="s">
-        <v>42</v>
+      <c r="G3" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="36"/>
+        <v>25</v>
+      </c>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="31"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -909,10 +907,10 @@
         <v>0</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="10" t="str">
         <f t="shared" ref="G5:G22" si="0">IF(AND(C5 = 0, D5=0, E5="No", F5="No"), "Yes", "No")</f>
@@ -934,10 +932,10 @@
         <v>0</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="8" t="str">
         <f t="shared" si="0"/>
@@ -959,10 +957,10 @@
         <v>0</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" s="8" t="str">
         <f t="shared" si="0"/>
@@ -984,10 +982,10 @@
         <v>0</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1009,10 +1007,10 @@
         <v>0</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G9" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1034,10 +1032,10 @@
         <v>0</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1059,10 +1057,10 @@
         <v>0</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G11" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1084,10 +1082,10 @@
         <v>0</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G12" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1109,10 +1107,10 @@
         <v>0</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G13" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1134,10 +1132,10 @@
         <v>0</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1159,10 +1157,10 @@
         <v>0</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G15" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1184,10 +1182,10 @@
         <v>0</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G16" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1209,10 +1207,10 @@
         <v>0</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G17" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1234,10 +1232,10 @@
         <v>0</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G18" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1259,10 +1257,10 @@
         <v>0</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G19" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1284,10 +1282,10 @@
         <v>0</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G20" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1309,10 +1307,10 @@
         <v>0</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G21" s="8" t="str">
         <f t="shared" si="0"/>
@@ -1334,10 +1332,10 @@
         <v>0</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G22" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1346,66 +1344,66 @@
       <c r="H22" s="9"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="21" t="s">
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="21" t="s">
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="21" t="s">
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="26"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="23"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="27"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="30"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="27"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="30"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="26"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B33" s="31"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="34"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1459,7 +1457,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1478,13 +1476,13 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
         <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1501,13 +1499,13 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1518,30 +1516,30 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -1549,13 +1547,13 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5">
         <v>3</v>

</xml_diff>